<commit_message>
Prompt changes and medgemma integration
</commit_message>
<xml_diff>
--- a/ontology/mcode_structure_modified.xlsx
+++ b/ontology/mcode_structure_modified.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/ningyuan_li_mail_mcgill_ca/Documents/research/masters/mcodegpt-streamlined-docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sven2\git-repo\mCodeGPT-streamlined\ontology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{0594FD4F-D6C2-4E22-9934-56458D0A748D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE181349-4D6F-404F-A79A-CC135BDDA177}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C31592-E79A-4634-B54D-EE48A9421597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{0015E88C-EFC2-4B52-ADE6-6746027C26F6}"/>
   </bookViews>
@@ -932,6 +932,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -950,13 +959,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -993,15 +1002,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1026,10 +1026,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1331,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3214E81-3B1F-4D6E-A390-A29A7543EC3B}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1361,10 +1357,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1373,23 +1369,23 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1397,7 +1393,7 @@
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1405,7 +1401,7 @@
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="27"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1413,7 +1409,7 @@
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="27"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1421,7 +1417,7 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1429,7 +1425,7 @@
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1437,7 +1433,7 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1445,7 +1441,7 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1453,7 +1449,7 @@
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1461,7 +1457,7 @@
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="27"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1471,8 +1467,8 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
-      <c r="B15" s="30" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1481,17 +1477,17 @@
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="27"/>
-      <c r="B16" s="30"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="27"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30" t="s">
+      <c r="A17" s="30"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1499,19 +1495,19 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
-      <c r="B19" s="32" t="s">
+      <c r="A19" s="30"/>
+      <c r="B19" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -1519,71 +1515,71 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="5" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="27"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="5" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="27"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="27"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="27"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="5" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="27"/>
-      <c r="B26" s="32"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="27"/>
-      <c r="B27" s="32"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="27"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
@@ -1591,8 +1587,8 @@
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="27"/>
-      <c r="B29" s="32" t="s">
+      <c r="A29" s="30"/>
+      <c r="B29" s="26" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -1601,16 +1597,16 @@
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="27"/>
-      <c r="B30" s="32"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28" t="s">
+      <c r="A31" s="30"/>
+      <c r="B31" s="31" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -1619,32 +1615,32 @@
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="27"/>
-      <c r="B35" s="28" t="s">
+      <c r="A35" s="30"/>
+      <c r="B35" s="31" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -1653,32 +1649,32 @@
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
-      <c r="B36" s="28"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="27"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="27"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28" t="s">
+      <c r="A39" s="30"/>
+      <c r="B39" s="31" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -1687,16 +1683,16 @@
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="27"/>
-      <c r="B40" s="28"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="27"/>
-      <c r="B41" s="28" t="s">
+      <c r="A41" s="30"/>
+      <c r="B41" s="31" t="s">
         <v>35</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -1705,63 +1701,63 @@
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="27"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="6" t="s">
         <v>215</v>
       </c>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="27"/>
-      <c r="B43" s="28"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="6" t="s">
         <v>216</v>
       </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="27"/>
-      <c r="B44" s="28"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="31"/>
       <c r="C44" s="6" t="s">
         <v>217</v>
       </c>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="27"/>
-      <c r="B45" s="28"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="31"/>
       <c r="C45" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="27"/>
-      <c r="B46" s="28"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="6" t="s">
         <v>218</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="27"/>
-      <c r="B47" s="28"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="6" t="s">
         <v>219</v>
       </c>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="27"/>
-      <c r="B48" s="28"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="27"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="7" t="s">
         <v>45</v>
       </c>
@@ -1769,7 +1765,7 @@
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="27"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="7" t="s">
         <v>46</v>
       </c>
@@ -1777,8 +1773,8 @@
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="27"/>
-      <c r="B51" s="29" t="s">
+      <c r="A51" s="30"/>
+      <c r="B51" s="32" t="s">
         <v>47</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -1787,16 +1783,16 @@
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="27"/>
-      <c r="B52" s="29"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="27"/>
-      <c r="B53" s="24" t="s">
+      <c r="A53" s="30"/>
+      <c r="B53" s="27" t="s">
         <v>54</v>
       </c>
       <c r="C53" s="9" t="s">
@@ -1804,92 +1800,92 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="27"/>
-      <c r="B54" s="25"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="27"/>
-      <c r="B55" s="25"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="27"/>
-      <c r="B56" s="25"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="27"/>
-      <c r="B57" s="25"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="27"/>
-      <c r="B58" s="25"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="27"/>
-      <c r="B59" s="25"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="27"/>
-      <c r="B60" s="25"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="27"/>
-      <c r="B61" s="25"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="27"/>
-      <c r="B62" s="25"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="27"/>
-      <c r="B63" s="25"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="27"/>
-      <c r="B64" s="25"/>
+      <c r="A64" s="30"/>
+      <c r="B64" s="28"/>
       <c r="C64" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="27"/>
-      <c r="B65" s="25"/>
+      <c r="A65" s="30"/>
+      <c r="B65" s="28"/>
       <c r="C65" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="27"/>
-      <c r="B66" s="25" t="s">
+      <c r="A66" s="30"/>
+      <c r="B66" s="28" t="s">
         <v>49</v>
       </c>
       <c r="C66" s="9" t="s">
@@ -1897,47 +1893,42 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="27"/>
-      <c r="B67" s="25"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="28"/>
       <c r="C67" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="27"/>
-      <c r="B68" s="25"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="28"/>
       <c r="C68" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="27"/>
-      <c r="B69" s="25"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="28"/>
       <c r="C69" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="27"/>
-      <c r="B70" s="25"/>
+      <c r="A70" s="30"/>
+      <c r="B70" s="28"/>
       <c r="C70" s="9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="27"/>
-      <c r="B71" s="25"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="28"/>
       <c r="C71" s="9" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B19:B27"/>
-    <mergeCell ref="C19:C24"/>
     <mergeCell ref="B53:B65"/>
     <mergeCell ref="B66:B71"/>
     <mergeCell ref="A2:A71"/>
@@ -1947,6 +1938,11 @@
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B19:B27"/>
+    <mergeCell ref="C19:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1956,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB56AD3A-0A0D-446C-845D-0E33FB16B9E5}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1983,10 +1979,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="44" t="s">
         <v>110</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1995,23 +1991,23 @@
       <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="31"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="2" t="s">
         <v>184</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="31"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="2" t="s">
         <v>185</v>
       </c>
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="2" t="s">
         <v>73</v>
       </c>
@@ -2019,7 +2015,7 @@
       <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="2" t="s">
         <v>186</v>
       </c>
@@ -2027,7 +2023,7 @@
       <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="2" t="s">
         <v>74</v>
       </c>
@@ -2035,7 +2031,7 @@
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="2" t="s">
         <v>75</v>
       </c>
@@ -2043,7 +2039,7 @@
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="31"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="2" t="s">
         <v>76</v>
       </c>
@@ -2051,7 +2047,7 @@
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="31"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="2" t="s">
         <v>187</v>
       </c>
@@ -2059,7 +2055,7 @@
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="31"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="2" t="s">
         <v>77</v>
       </c>
@@ -2067,7 +2063,7 @@
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="31"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="2" t="s">
         <v>78</v>
       </c>
@@ -2075,7 +2071,7 @@
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="31"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="14" t="s">
         <v>188</v>
       </c>
@@ -2083,7 +2079,7 @@
       <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="31"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="14" t="s">
         <v>111</v>
       </c>
@@ -2093,8 +2089,8 @@
       <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="42" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="45" t="s">
         <v>112</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -2103,17 +2099,17 @@
       <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="43"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="4" t="s">
         <v>191</v>
       </c>
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="31"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="30" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="24" t="s">
         <v>79</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -2121,19 +2117,19 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="31"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="30"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="11" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="31"/>
-      <c r="B19" s="45" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="26" t="s">
         <v>114</v>
       </c>
       <c r="D19" s="12" t="s">
@@ -2141,71 +2137,71 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="31"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="32"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="12" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="32"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="12" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="32"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="12" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="31"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="32"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="12" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="32"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="12" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="31"/>
-      <c r="B25" s="46"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
-      <c r="B26" s="46"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="34"/>
       <c r="C26" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="31"/>
-      <c r="B27" s="47"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="5" t="s">
         <v>208</v>
       </c>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="31"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="15" t="s">
         <v>206</v>
       </c>
@@ -2213,8 +2209,8 @@
       <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="31"/>
-      <c r="B29" s="45" t="s">
+      <c r="A29" s="25"/>
+      <c r="B29" s="33" t="s">
         <v>115</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -2223,16 +2219,16 @@
       <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="31"/>
-      <c r="B30" s="47"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="31"/>
-      <c r="B31" s="33" t="s">
+      <c r="A31" s="25"/>
+      <c r="B31" s="36" t="s">
         <v>116</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -2241,32 +2237,32 @@
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="31"/>
-      <c r="B32" s="34"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="6" t="s">
         <v>210</v>
       </c>
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="31"/>
-      <c r="B33" s="34"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="37"/>
       <c r="C33" s="6" t="s">
         <v>83</v>
       </c>
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="31"/>
-      <c r="B34" s="35"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="31"/>
-      <c r="B35" s="33" t="s">
+      <c r="A35" s="25"/>
+      <c r="B35" s="36" t="s">
         <v>117</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -2275,32 +2271,32 @@
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="31"/>
-      <c r="B36" s="34"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="6" t="s">
         <v>212</v>
       </c>
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="31"/>
-      <c r="B37" s="34"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="37"/>
       <c r="C37" s="6" t="s">
         <v>85</v>
       </c>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="31"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="38"/>
       <c r="C38" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="31"/>
-      <c r="B39" s="33" t="s">
+      <c r="A39" s="25"/>
+      <c r="B39" s="36" t="s">
         <v>118</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -2309,16 +2305,16 @@
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="31"/>
-      <c r="B40" s="35"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="6" t="s">
         <v>214</v>
       </c>
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="31"/>
-      <c r="B41" s="33" t="s">
+      <c r="A41" s="25"/>
+      <c r="B41" s="36" t="s">
         <v>119</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -2327,63 +2323,63 @@
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="31"/>
-      <c r="B42" s="34"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="6" t="s">
         <v>221</v>
       </c>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="31"/>
-      <c r="B43" s="34"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="37"/>
       <c r="C43" s="6" t="s">
         <v>222</v>
       </c>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="31"/>
-      <c r="B44" s="34"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="37"/>
       <c r="C44" s="6" t="s">
         <v>223</v>
       </c>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="31"/>
-      <c r="B45" s="34"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="37"/>
       <c r="C45" s="6" t="s">
         <v>224</v>
       </c>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="31"/>
-      <c r="B46" s="34"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="37"/>
       <c r="C46" s="6" t="s">
         <v>225</v>
       </c>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="31"/>
-      <c r="B47" s="34"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="6" t="s">
         <v>226</v>
       </c>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="31"/>
-      <c r="B48" s="35"/>
+      <c r="A48" s="25"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="6" t="s">
         <v>227</v>
       </c>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A49" s="31"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="16" t="s">
         <v>87</v>
       </c>
@@ -2391,7 +2387,7 @@
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A50" s="31"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="16" t="s">
         <v>88</v>
       </c>
@@ -2399,8 +2395,8 @@
       <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="31"/>
-      <c r="B51" s="36" t="s">
+      <c r="A51" s="25"/>
+      <c r="B51" s="39" t="s">
         <v>120</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -2409,16 +2405,16 @@
       <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="31"/>
-      <c r="B52" s="37"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="31"/>
-      <c r="B53" s="38" t="s">
+      <c r="A53" s="25"/>
+      <c r="B53" s="41" t="s">
         <v>121</v>
       </c>
       <c r="C53" s="17" t="s">
@@ -2427,104 +2423,104 @@
       <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="31"/>
-      <c r="B54" s="39"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="42"/>
       <c r="C54" s="17" t="s">
         <v>92</v>
       </c>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="31"/>
-      <c r="B55" s="39"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="42"/>
       <c r="C55" s="17" t="s">
         <v>93</v>
       </c>
       <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="31"/>
-      <c r="B56" s="39"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="42"/>
       <c r="C56" s="17" t="s">
         <v>94</v>
       </c>
       <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="31"/>
-      <c r="B57" s="39"/>
+      <c r="A57" s="25"/>
+      <c r="B57" s="42"/>
       <c r="C57" s="17" t="s">
         <v>95</v>
       </c>
       <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="31"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="42"/>
       <c r="C58" s="17" t="s">
         <v>96</v>
       </c>
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="31"/>
-      <c r="B59" s="39"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="42"/>
       <c r="C59" s="17" t="s">
         <v>97</v>
       </c>
       <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="31"/>
-      <c r="B60" s="39"/>
+      <c r="A60" s="25"/>
+      <c r="B60" s="42"/>
       <c r="C60" s="17" t="s">
         <v>98</v>
       </c>
       <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="31"/>
-      <c r="B61" s="39"/>
+      <c r="A61" s="25"/>
+      <c r="B61" s="42"/>
       <c r="C61" s="17" t="s">
         <v>99</v>
       </c>
       <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="31"/>
-      <c r="B62" s="39"/>
+      <c r="A62" s="25"/>
+      <c r="B62" s="42"/>
       <c r="C62" s="17" t="s">
         <v>100</v>
       </c>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="31"/>
-      <c r="B63" s="39"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="42"/>
       <c r="C63" s="17" t="s">
         <v>101</v>
       </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="31"/>
-      <c r="B64" s="39"/>
+      <c r="A64" s="25"/>
+      <c r="B64" s="42"/>
       <c r="C64" s="17" t="s">
         <v>102</v>
       </c>
       <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="31"/>
-      <c r="B65" s="40"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="43"/>
       <c r="C65" s="17" t="s">
         <v>103</v>
       </c>
       <c r="D65" s="1"/>
     </row>
     <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="31"/>
-      <c r="B66" s="38" t="s">
+      <c r="A66" s="25"/>
+      <c r="B66" s="41" t="s">
         <v>122</v>
       </c>
       <c r="C66" s="17" t="s">
@@ -2533,40 +2529,40 @@
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="31"/>
-      <c r="B67" s="39"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="42"/>
       <c r="C67" s="17" t="s">
         <v>105</v>
       </c>
       <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="31"/>
-      <c r="B68" s="39"/>
+      <c r="A68" s="25"/>
+      <c r="B68" s="42"/>
       <c r="C68" s="17" t="s">
         <v>106</v>
       </c>
       <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" s="31"/>
-      <c r="B69" s="39"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="42"/>
       <c r="C69" s="17" t="s">
         <v>107</v>
       </c>
       <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="31"/>
-      <c r="B70" s="39"/>
+      <c r="A70" s="25"/>
+      <c r="B70" s="42"/>
       <c r="C70" s="17" t="s">
         <v>108</v>
       </c>
       <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="31"/>
-      <c r="B71" s="40"/>
+      <c r="A71" s="25"/>
+      <c r="B71" s="43"/>
       <c r="C71" s="17" t="s">
         <v>109</v>
       </c>
@@ -2574,11 +2570,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B27"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B34"/>
     <mergeCell ref="B41:B48"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B53:B65"/>
@@ -2588,6 +2579,11 @@
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B27"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2599,7 +2595,7 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2625,31 +2621,31 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="31"/>
-      <c r="B2" s="41"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="18" t="s">
         <v>124</v>
       </c>
       <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="31"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="18" t="s">
         <v>125</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="31"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="18" t="s">
         <v>126</v>
       </c>
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="18" t="s">
         <v>127</v>
       </c>
@@ -2657,7 +2653,7 @@
       <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="18" t="s">
         <v>128</v>
       </c>
@@ -2665,7 +2661,7 @@
       <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="18" t="s">
         <v>129</v>
       </c>
@@ -2673,7 +2669,7 @@
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="18" t="s">
         <v>130</v>
       </c>
@@ -2681,7 +2677,7 @@
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="31"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="18" t="s">
         <v>131</v>
       </c>
@@ -2689,7 +2685,7 @@
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="31"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="18" t="s">
         <v>132</v>
       </c>
@@ -2697,7 +2693,7 @@
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="31"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="18" t="s">
         <v>133</v>
       </c>
@@ -2705,7 +2701,7 @@
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="31"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="18" t="s">
         <v>134</v>
       </c>
@@ -2713,7 +2709,7 @@
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="31"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="18" t="s">
         <v>135</v>
       </c>
@@ -2721,7 +2717,7 @@
       <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="31"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="14"/>
       <c r="C14" s="19" t="s">
         <v>136</v>
@@ -2729,131 +2725,131 @@
       <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="42"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="19" t="s">
         <v>137</v>
       </c>
       <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="43"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="19" t="s">
         <v>138</v>
       </c>
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="31"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="30"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="19" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="31"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="30"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="19" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="31"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="32"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="20" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="31"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="32"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="20"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="32"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="32"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="20"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="31"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="32"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="20"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="32"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="20"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="31"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="32"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="20"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="32"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="20"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="31"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="32"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="20"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="31"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="32"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="20"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="31"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="32"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="20"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="31"/>
-      <c r="B30" s="46"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="20" t="s">
         <v>141</v>
       </c>
       <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="31"/>
-      <c r="B31" s="46"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="20" t="s">
         <v>142</v>
       </c>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="31"/>
-      <c r="B32" s="47"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="20" t="s">
         <v>143</v>
       </c>
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="31"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="20" t="s">
         <v>144</v>
       </c>
@@ -2861,127 +2857,127 @@
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="31"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="20" t="s">
         <v>145</v>
       </c>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="31"/>
-      <c r="B35" s="47"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="20" t="s">
         <v>146</v>
       </c>
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="31"/>
-      <c r="B36" s="33"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="21" t="s">
         <v>147</v>
       </c>
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="31"/>
-      <c r="B37" s="34"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="37"/>
       <c r="C37" s="21" t="s">
         <v>148</v>
       </c>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="31"/>
-      <c r="B38" s="34"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="37"/>
       <c r="C38" s="21" t="s">
         <v>149</v>
       </c>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="31"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="38"/>
       <c r="C39" s="21" t="s">
         <v>150</v>
       </c>
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="31"/>
-      <c r="B40" s="33"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="36"/>
       <c r="C40" s="21" t="s">
         <v>151</v>
       </c>
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="31"/>
-      <c r="B41" s="34"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="21" t="s">
         <v>152</v>
       </c>
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="31"/>
-      <c r="B42" s="34"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="21" t="s">
         <v>153</v>
       </c>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="31"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="38"/>
       <c r="C43" s="21" t="s">
         <v>154</v>
       </c>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="31"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="21" t="s">
         <v>155</v>
       </c>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="31"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="21" t="s">
         <v>156</v>
       </c>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="31"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="21" t="s">
         <v>157</v>
       </c>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="31"/>
-      <c r="B47" s="34"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="21" t="s">
         <v>158</v>
       </c>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="31"/>
-      <c r="B48" s="35"/>
+      <c r="A48" s="25"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="21" t="s">
         <v>159</v>
       </c>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="31"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="22" t="s">
         <v>160</v>
       </c>
@@ -2989,7 +2985,7 @@
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="31"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="22" t="s">
         <v>161</v>
       </c>
@@ -2997,168 +2993,168 @@
       <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="31"/>
-      <c r="B51" s="36"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="39"/>
       <c r="C51" s="22" t="s">
         <v>162</v>
       </c>
       <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="31"/>
-      <c r="B52" s="37"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="22" t="s">
         <v>163</v>
       </c>
       <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="31"/>
-      <c r="B53" s="38"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="41"/>
       <c r="C53" s="23" t="s">
         <v>164</v>
       </c>
       <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="31"/>
-      <c r="B54" s="39"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="42"/>
       <c r="C54" s="23" t="s">
         <v>165</v>
       </c>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="31"/>
-      <c r="B55" s="39"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="42"/>
       <c r="C55" s="23" t="s">
         <v>166</v>
       </c>
       <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="31"/>
-      <c r="B56" s="39"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="42"/>
       <c r="C56" s="23" t="s">
         <v>167</v>
       </c>
       <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="31"/>
-      <c r="B57" s="39"/>
+      <c r="A57" s="25"/>
+      <c r="B57" s="42"/>
       <c r="C57" s="23" t="s">
         <v>168</v>
       </c>
       <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="31"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="42"/>
       <c r="C58" s="23" t="s">
         <v>169</v>
       </c>
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="31"/>
-      <c r="B59" s="39"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="42"/>
       <c r="C59" s="23" t="s">
         <v>170</v>
       </c>
       <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="31"/>
-      <c r="B60" s="39"/>
+      <c r="A60" s="25"/>
+      <c r="B60" s="42"/>
       <c r="C60" s="23" t="s">
         <v>171</v>
       </c>
       <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="31"/>
-      <c r="B61" s="39"/>
+      <c r="A61" s="25"/>
+      <c r="B61" s="42"/>
       <c r="C61" s="23" t="s">
         <v>172</v>
       </c>
       <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="31"/>
-      <c r="B62" s="39"/>
+      <c r="A62" s="25"/>
+      <c r="B62" s="42"/>
       <c r="C62" s="23" t="s">
         <v>173</v>
       </c>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="31"/>
-      <c r="B63" s="39"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="42"/>
       <c r="C63" s="23" t="s">
         <v>174</v>
       </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="31"/>
-      <c r="B64" s="39"/>
+      <c r="A64" s="25"/>
+      <c r="B64" s="42"/>
       <c r="C64" s="23" t="s">
         <v>175</v>
       </c>
       <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="31"/>
-      <c r="B65" s="40"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="43"/>
       <c r="C65" s="23" t="s">
         <v>176</v>
       </c>
       <c r="D65" s="1"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="31"/>
-      <c r="B66" s="38"/>
+      <c r="A66" s="25"/>
+      <c r="B66" s="41"/>
       <c r="C66" s="23" t="s">
         <v>177</v>
       </c>
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="31"/>
-      <c r="B67" s="39"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="42"/>
       <c r="C67" s="23" t="s">
         <v>178</v>
       </c>
       <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="31"/>
-      <c r="B68" s="39"/>
+      <c r="A68" s="25"/>
+      <c r="B68" s="42"/>
       <c r="C68" s="23" t="s">
         <v>179</v>
       </c>
       <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" s="31"/>
-      <c r="B69" s="39"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="42"/>
       <c r="C69" s="23" t="s">
         <v>180</v>
       </c>
       <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="31"/>
-      <c r="B70" s="39"/>
+      <c r="A70" s="25"/>
+      <c r="B70" s="42"/>
       <c r="C70" s="23" t="s">
         <v>181</v>
       </c>
       <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="31"/>
-      <c r="B71" s="40"/>
+      <c r="A71" s="25"/>
+      <c r="B71" s="43"/>
       <c r="C71" s="23" t="s">
         <v>182</v>
       </c>
@@ -3166,6 +3162,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B32"/>
+    <mergeCell ref="C19:C29"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B39"/>
     <mergeCell ref="B46:B48"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B53:B65"/>
@@ -3175,11 +3176,6 @@
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B32"/>
-    <mergeCell ref="C19:C29"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>